<commit_message>
Updated H2 and CCS models
</commit_message>
<xml_diff>
--- a/data/i2cner-tech-data.xlsx
+++ b/data/i2cner-tech-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achubbz\Documents\GitHub\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{45259D84-3474-4E0E-B8C5-7D2C01FF17C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{04528D74-49AA-41C6-89A4-00F9A8BD279E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="1" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="2" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CCS" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="106">
   <si>
     <t>H2 Method</t>
   </si>
@@ -237,9 +237,6 @@
     <t>300 Nm3/h</t>
   </si>
   <si>
-    <t>Unit Cost( JPY/unit)</t>
-  </si>
-  <si>
     <t>Total Cost</t>
   </si>
   <si>
@@ -343,6 +340,12 @@
   </si>
   <si>
     <t>No data</t>
+  </si>
+  <si>
+    <t>Cost( JPY/unit)</t>
+  </si>
+  <si>
+    <t>ELC share</t>
   </si>
 </sst>
 </file>
@@ -1105,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47851EB-8A83-4629-AF5F-F0859B72869A}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,10 +1175,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
         <v>75</v>
-      </c>
-      <c r="B4" t="s">
-        <v>76</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="1"/>
@@ -1250,131 +1253,134 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26522F16-178D-4C9D-9097-E5B0FFBFDA90}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.21875" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" customWidth="1"/>
-    <col min="13" max="13" width="15.21875" customWidth="1"/>
-    <col min="14" max="14" width="13.44140625" customWidth="1"/>
-    <col min="15" max="15" width="16.21875" customWidth="1"/>
-    <col min="16" max="16" width="15.109375" customWidth="1"/>
-    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.21875" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.21875" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" customWidth="1"/>
+    <col min="16" max="16" width="16.21875" customWidth="1"/>
+    <col min="17" max="17" width="15.109375" customWidth="1"/>
+    <col min="18" max="18" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>65</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>39444.433400000002</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>68</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="5">
+      <c r="I2" s="5">
         <f>70.8/(1.8*1000000000)</f>
         <v>3.9333333333333335E-8</v>
       </c>
-      <c r="I2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="J2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L2" t="s">
         <v>67</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>8.8999999999999999E-3</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>93</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1391,45 +1397,49 @@
         <v>2.2481153767984923</v>
       </c>
       <c r="E5">
+        <f>D5/D9</f>
+        <v>0.66328485235107681</v>
+      </c>
+      <c r="F5">
         <v>114000</v>
       </c>
-      <c r="F5">
-        <f>E5*B5*$M$2/1000000</f>
+      <c r="G5">
+        <f>F5*B5*$N$2/1000000</f>
         <v>0.44834159400000001</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>14</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1538396</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <f>C9*0.7</f>
         <v>5.5676052871483162</v>
       </c>
-      <c r="L5">
-        <f>K6/H6</f>
+      <c r="M5">
+        <f>L6/I6</f>
         <v>30.363615543241984</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="N5" t="s">
-        <v>95</v>
-      </c>
-      <c r="O5">
-        <f>186/K6</f>
+      <c r="N5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O5" t="s">
+        <v>94</v>
+      </c>
+      <c r="P5">
+        <f>186/L6</f>
         <v>101.2349716919415</v>
       </c>
-      <c r="P5">
-        <f>(F9-G16)/K6</f>
+      <c r="Q5">
+        <f>(G9-G16)/L6</f>
         <v>0.24122779924311022</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1437,40 +1447,40 @@
         <f>3428</f>
         <v>3428</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>300</v>
       </c>
-      <c r="F6">
-        <f>E6*B6*$M$2/1000000</f>
+      <c r="G6">
+        <f>F6*B6*$N$2/1000000</f>
         <v>9.1527599999999994E-3</v>
       </c>
-      <c r="H6">
-        <f>(H5*H2)</f>
+      <c r="I6">
+        <f>(I5*I2)</f>
         <v>6.0510242666666672E-2</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>42</v>
       </c>
-      <c r="J6" t="s">
-        <v>81</v>
-      </c>
-      <c r="K6" s="6">
-        <f>0.33*K5</f>
+      <c r="K6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="6">
+        <f>0.33*L5</f>
         <v>1.8373097447589444</v>
       </c>
-      <c r="M6" t="s">
-        <v>86</v>
-      </c>
-      <c r="N6">
+      <c r="N6" t="s">
+        <v>85</v>
+      </c>
+      <c r="O6">
         <f>87/(1000000*0.27777)</f>
         <v>3.1320876984555567E-4</v>
       </c>
-      <c r="O6">
-        <f>O5*M2</f>
+      <c r="P6">
+        <f>P5*N2</f>
         <v>0.90099124805827935</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1478,29 +1488,29 @@
         <f>1714</f>
         <v>1714</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>200</v>
       </c>
-      <c r="F7">
-        <f>E7*B7*$M$2/1000000</f>
+      <c r="G7">
+        <f>F7*B7*$N$2/1000000</f>
         <v>3.0509199999999999E-3</v>
       </c>
-      <c r="H7">
-        <f>F1*H6</f>
+      <c r="I7">
+        <f>G1*I6</f>
         <v>2386.7922368831719</v>
       </c>
-      <c r="I7" t="s">
-        <v>97</v>
-      </c>
       <c r="J7" t="s">
-        <v>87</v>
-      </c>
-      <c r="M7">
-        <f>K6/D9</f>
+        <v>96</v>
+      </c>
+      <c r="K7" t="s">
+        <v>86</v>
+      </c>
+      <c r="N7">
+        <f>L6/D9</f>
         <v>0.54208059575265499</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1516,14 +1526,18 @@
         <v>1.141251</v>
       </c>
       <c r="E8">
+        <f>D8/D9</f>
+        <v>0.33671514764892313</v>
+      </c>
+      <c r="F8">
         <v>16</v>
       </c>
-      <c r="F8">
-        <f>E8*B8*$M$2/1000000</f>
+      <c r="G8">
+        <f>F8*B8*$N$2/1000000</f>
         <v>0.16251414240000001</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C9">
         <f>SUM(C5:C8)</f>
         <v>7.9537218387833093</v>
@@ -1532,31 +1546,31 @@
         <f>SUM(D5:D8)</f>
         <v>3.3893663767984923</v>
       </c>
-      <c r="F9">
-        <f>SUM(F5:F8)</f>
+      <c r="G9">
+        <f>SUM(G5:G8)</f>
         <v>0.62305941640000007</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" t="s">
         <v>78</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11">
+        <f>60*N2/(1000000*I2*M5)</f>
+        <v>0.44712301033802088</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>79</v>
-      </c>
-      <c r="F11">
-        <f>60*M2/(1000000*H2*L5)</f>
-        <v>0.44712301033802088</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>80</v>
       </c>
       <c r="B14">
         <v>55.5</v>
@@ -1565,19 +1579,19 @@
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15">
         <f>55.5*0.277777778</f>
         <v>15.416666678999999</v>
@@ -1586,19 +1600,19 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15">
-        <f>F5/D5</f>
+        <f>G5/D5</f>
         <v>0.19942997527043146</v>
       </c>
       <c r="F15">
         <v>0.44834159400000001</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E16">
         <v>0.08</v>
@@ -1632,28 +1646,28 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C1">
         <v>2050</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
         <v>100</v>
-      </c>
-      <c r="E2" t="s">
-        <v>101</v>
       </c>
       <c r="F2">
         <f>9/(39.4*0.3)</f>
         <v>0.76142131979695438</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1661,22 +1675,22 @@
         <v>2050</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F3">
         <f>1.5/(39.444*0.3)</f>
         <v>0.12676199168441335</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" t="s">
         <v>103</v>
-      </c>
-      <c r="C5" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated emissions and input of steam reforming H2
Former-commit-id: bff16133148454026e03aa49091f80a05e330f2e [formerly b3af39330800e2cef5c8ea85310adff8e3acb250]
Former-commit-id: 53863e4460514a0e47de82ea52a23cf6c888ff19
</commit_message>
<xml_diff>
--- a/data/i2cner-tech-data.xlsx
+++ b/data/i2cner-tech-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achubbz\Documents\GitHub\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{04528D74-49AA-41C6-89A4-00F9A8BD279E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2254764E-2B08-4F40-A8F0-884726151901}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="2" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="107">
   <si>
     <t>H2 Method</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>ELC share</t>
+  </si>
+  <si>
+    <t>ELC/LNG:</t>
   </si>
 </sst>
 </file>
@@ -1447,6 +1450,10 @@
         <f>3428</f>
         <v>3428</v>
       </c>
+      <c r="E6">
+        <f>D8/D9</f>
+        <v>0.33671514764892313</v>
+      </c>
       <c r="F6">
         <v>300</v>
       </c>
@@ -1488,6 +1495,9 @@
         <f>1714</f>
         <v>1714</v>
       </c>
+      <c r="E7" t="s">
+        <v>106</v>
+      </c>
       <c r="F7">
         <v>200</v>
       </c>
@@ -1526,8 +1536,8 @@
         <v>1.141251</v>
       </c>
       <c r="E8">
-        <f>D8/D9</f>
-        <v>0.33671514764892313</v>
+        <f>D8/D5</f>
+        <v>0.50764787776383546</v>
       </c>
       <c r="F8">
         <v>16</v>
@@ -1628,6 +1638,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated steam reforming efficiency value
</commit_message>
<xml_diff>
--- a/data/i2cner-tech-data.xlsx
+++ b/data/i2cner-tech-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achubbz\Documents\GitHub\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2254764E-2B08-4F40-A8F0-884726151901}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8A87543A-5948-4776-8883-C8F5A5308814}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="2" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="108">
   <si>
     <t>H2 Method</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>ELC/LNG:</t>
+  </si>
+  <si>
+    <t>LNG input only:</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1262,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1546,6 +1549,9 @@
         <f>F8*B8*$N$2/1000000</f>
         <v>0.16251414240000001</v>
       </c>
+      <c r="N8" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C9">
@@ -1559,6 +1565,10 @@
       <c r="G9">
         <f>SUM(G5:G8)</f>
         <v>0.62305941640000007</v>
+      </c>
+      <c r="N9">
+        <f>L6/D5</f>
+        <v>0.81726665976344592</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added co2 emissions for h2
Former-commit-id: 26b4ed267405d397bab859897d4eb1252cc68582 [formerly 04fa42813d9fdfbaaa741ffb8aa11d1caca47061]
Former-commit-id: 8ebcbf5963f8f34db53a95077832094d45998d43
</commit_message>
<xml_diff>
--- a/data/i2cner-tech-data.xlsx
+++ b/data/i2cner-tech-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achubbz\Documents\GitHub\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E6865086-ABC1-43C1-A030-F71CEFA5078A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1F272FF2-8FD1-4B48-8ABC-D381F144C189}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" firstSheet="1" activeTab="3" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CCS" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="118">
   <si>
     <t>H2 Method</t>
   </si>
@@ -373,6 +373,15 @@
   </si>
   <si>
     <t>New Emi(Mt/GWh)</t>
+  </si>
+  <si>
+    <t>based on competitive cost of h2/elc projections</t>
+  </si>
+  <si>
+    <t>No emissions due to high energy density, uses less steel/concrete than nuclear</t>
+  </si>
+  <si>
+    <t>no data on emissions intensity anyway :(</t>
   </si>
 </sst>
 </file>
@@ -806,7 +815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C7BE1D-16BA-4023-AA64-49E118FA5EEE}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="N8" sqref="N8:N10"/>
     </sheetView>
   </sheetViews>
@@ -1788,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D8D9EFC-D052-4551-86BD-609CA1895FF2}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1799,7 +1808,7 @@
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>97</v>
       </c>
@@ -1810,7 +1819,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>99</v>
       </c>
@@ -1825,7 +1834,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D3">
         <v>2050</v>
       </c>
@@ -1839,13 +1848,24 @@
       <c r="G3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>102</v>
       </c>
       <c r="C5" t="s">
         <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added CCS seam reforming data
Former-commit-id: a249ef23e422e6d8fdf7522884a1b64b98e80487
Former-commit-id: a68fb94a5b731b00891dd65c2c1bfdc20f89ae62
</commit_message>
<xml_diff>
--- a/data/i2cner-tech-data.xlsx
+++ b/data/i2cner-tech-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF4EE17-D02A-4AC3-8CA1-11C61F263665}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F730DAAD-5F76-409C-A4C2-30821CBECAAB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33780" yWindow="3360" windowWidth="11520" windowHeight="12360" firstSheet="5" activeTab="6" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CCS" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Photocatalytic H2" sheetId="4" r:id="rId5"/>
     <sheet name="Kato_H2" sheetId="7" r:id="rId6"/>
     <sheet name="Keipi_SMR" sheetId="5" r:id="rId7"/>
-    <sheet name="Keipi_electrolysis" sheetId="8" r:id="rId8"/>
+    <sheet name="KEIPI_CCSSMR" sheetId="9" r:id="rId8"/>
+    <sheet name="Keipi_electrolysis" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="214">
   <si>
     <t>H2 Method</t>
   </si>
@@ -665,6 +666,21 @@
   </si>
   <si>
     <t>added to make unit price match the paper</t>
+  </si>
+  <si>
+    <t>CCS cost</t>
+  </si>
+  <si>
+    <t>EUR/MWh-H2</t>
+  </si>
+  <si>
+    <t>CCS ELC</t>
+  </si>
+  <si>
+    <t>CCSELC</t>
+  </si>
+  <si>
+    <t>Total /yr</t>
   </si>
 </sst>
 </file>
@@ -809,11 +825,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1135,20 +1151,20 @@
       <selection activeCell="N8" sqref="N8:N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -1169,7 +1185,7 @@
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>48</v>
       </c>
@@ -1189,7 +1205,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>2030</v>
       </c>
@@ -1203,7 +1219,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2050</v>
       </c>
@@ -1218,10 +1234,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>47</v>
       </c>
@@ -1241,7 +1257,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="J7" t="s">
         <v>104</v>
@@ -1259,7 +1275,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -1297,7 +1313,7 @@
         <v>4.8029415295134311E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="C9" t="s">
         <v>40</v>
@@ -1330,7 +1346,7 @@
         <v>3.0302435280682926E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -1365,7 +1381,7 @@
         <v>3.7436445981853416E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -1376,7 +1392,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1398,7 +1414,7 @@
         <v>0.11883889324915139</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="D13" s="7">
         <f>D12*K1</f>
@@ -1412,7 +1428,7 @@
         <v>0.18835986296837956</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" t="s">
         <v>49</v>
@@ -1429,7 +1445,7 @@
         <v>0.15246539588304808</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D15" s="6">
         <f>D14*K1</f>
         <v>19.416682200000004</v>
@@ -1438,7 +1454,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>55</v>
       </c>
@@ -1456,7 +1472,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>36</v>
       </c>
@@ -1471,7 +1487,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
@@ -1486,7 +1502,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -1500,7 +1516,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>57</v>
       </c>
@@ -1515,7 +1531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>47</v>
       </c>
@@ -1533,7 +1549,7 @@
         <v>40.840000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>58</v>
       </c>
@@ -1551,7 +1567,7 @@
         <v>36.49</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>55</v>
       </c>
@@ -1574,26 +1590,26 @@
   <dimension ref="A2:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:N5"/>
+      <selection activeCell="G3" sqref="G3:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="2" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1614,7 +1630,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1635,7 +1651,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
         <v>1</v>
       </c>
@@ -1667,7 +1683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>123</v>
       </c>
@@ -1685,7 +1701,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>68</v>
       </c>
@@ -1701,7 +1717,7 @@
       <c r="L7" s="12"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="K8" t="s">
         <v>127</v>
       </c>
@@ -1719,7 +1735,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>122</v>
       </c>
@@ -1741,7 +1757,7 @@
       </c>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10">
         <f>B9*K2</f>
         <v>1690909.0909090908</v>
@@ -1763,10 +1779,10 @@
       <c r="G10" t="s">
         <v>139</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="K10" s="14"/>
+      <c r="K10" s="16"/>
       <c r="L10" s="12">
         <f>L9/G5</f>
         <v>122583.35123523093</v>
@@ -1775,11 +1791,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J11" s="14" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J11" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="K11" s="14"/>
+      <c r="K11" s="16"/>
       <c r="L11" s="12">
         <f>M4*L10</f>
         <v>4086438.5967776584</v>
@@ -1795,7 +1811,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>144</v>
       </c>
@@ -1810,7 +1826,7 @@
       </c>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1840,7 +1856,7 @@
       </c>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>118</v>
       </c>
@@ -1865,7 +1881,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>119</v>
       </c>
@@ -1890,7 +1906,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1907,7 +1923,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>134</v>
       </c>
@@ -1920,12 +1936,12 @@
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>146</v>
       </c>
@@ -1937,7 +1953,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>148</v>
       </c>
@@ -1950,7 +1966,7 @@
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>151</v>
       </c>
@@ -1962,7 +1978,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>152</v>
       </c>
@@ -1980,7 +1996,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2009,7 +2025,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>154</v>
       </c>
@@ -2025,19 +2041,19 @@
         <v>1979999.1818181819</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G26">
         <f>F16*20</f>
         <v>258468265.45454544</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I27">
         <f>SUM(G24:G26)/(L10*20)</f>
         <v>106.92282886941211</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="G28">
         <f>SUM(G24:G26)/I24</f>
@@ -2047,7 +2063,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>140</v>
       </c>
@@ -2065,7 +2081,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -2095,9 +2111,9 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>123</v>
       </c>
@@ -2111,7 +2127,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>159</v>
       </c>
@@ -2135,23 +2151,23 @@
       <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" customWidth="1"/>
-    <col min="17" max="17" width="15.140625" customWidth="1"/>
+    <col min="4" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" customWidth="1"/>
+    <col min="17" max="17" width="15.109375" customWidth="1"/>
     <col min="18" max="18" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>59</v>
       </c>
@@ -2162,7 +2178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -2189,7 +2205,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2207,7 +2223,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -2256,7 +2272,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2315,7 +2331,7 @@
         <v>0.24122779924311022</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2360,7 +2376,7 @@
         <v>0.90099124805827935</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2393,7 +2409,7 @@
         <v>0.54208059575265499</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2423,7 +2439,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C9">
         <f>SUM(C5:C8)</f>
         <v>7.9537218387833093</v>
@@ -2441,7 +2457,7 @@
         <v>0.81726665976344592</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>70</v>
       </c>
@@ -2453,12 +2469,12 @@
         <v>0.44712301033802088</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2481,7 +2497,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15">
         <f>55.5*0.277777778</f>
         <v>15.416666678999999</v>
@@ -2500,7 +2516,7 @@
         <v>0.44834159400000001</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>82</v>
       </c>
@@ -2530,12 +2546,12 @@
       <selection activeCell="E24" sqref="E24:F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -2546,7 +2562,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>92</v>
       </c>
@@ -2561,7 +2577,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D3">
         <v>2050</v>
       </c>
@@ -2579,7 +2595,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -2590,7 +2606,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>110</v>
       </c>
@@ -2605,16 +2621,16 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D18" sqref="D18:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>161</v>
       </c>
@@ -2625,12 +2641,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2641,7 +2657,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -2659,12 +2675,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2672,7 +2688,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -2690,7 +2706,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>141</v>
       </c>
@@ -2710,22 +2726,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5DFEF8-915B-4056-B382-3EF1CD6D8429}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C1" s="5">
         <v>41.869</v>
       </c>
@@ -2749,7 +2765,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="10">
@@ -2765,7 +2781,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2797,7 +2813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -2815,18 +2831,18 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>207</v>
       </c>
       <c r="C6">
         <v>0.65</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>168</v>
       </c>
@@ -2858,7 +2874,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>171</v>
       </c>
@@ -2884,7 +2900,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
@@ -2895,7 +2911,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>174</v>
       </c>
@@ -2915,7 +2931,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>175</v>
       </c>
@@ -2952,7 +2968,7 @@
         <v>1.1486621432696928E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>176</v>
       </c>
@@ -2976,10 +2992,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>177</v>
       </c>
@@ -2997,7 +3013,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>181</v>
       </c>
@@ -3008,7 +3024,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>B19*(365*24*60*60)</f>
         <v>378432000</v>
@@ -3017,7 +3033,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21">
         <f>B20*0.3</f>
         <v>113529600</v>
@@ -3040,7 +3056,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>186</v>
       </c>
@@ -3066,12 +3082,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>185</v>
       </c>
@@ -3097,10 +3113,10 @@
         <v>188</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="15"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>192</v>
       </c>
@@ -3112,7 +3128,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>195</v>
       </c>
@@ -3124,7 +3140,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>197</v>
       </c>
@@ -3143,22 +3159,553 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AA85B1-F75D-401E-9CDA-9DC2F24930C6}">
+  <dimension ref="A1:O38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C1" s="5">
+        <v>41.869</v>
+      </c>
+      <c r="D1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1">
+        <f>1/110</f>
+        <v>9.0909090909090905E-3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="10">
+        <v>0.27779999999999999</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <f>C3*C1</f>
+        <v>5024.28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3">
+        <f>C2*E3</f>
+        <v>1395.7449839999999</v>
+      </c>
+      <c r="H3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3">
+        <f>C3*C2</f>
+        <v>33.335999999999999</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4">
+        <v>9.31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4">
+        <f>C4/I3</f>
+        <v>0.27927765778737701</v>
+      </c>
+      <c r="F4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6">
+        <v>0.65</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8">
+        <v>2.5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8">
+        <f>B8*(365*24*60*60)</f>
+        <v>78840000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8">
+        <f>(D8*I3*C6/(1000000))</f>
+        <v>1708.3366559999999</v>
+      </c>
+      <c r="G8" t="s">
+        <v>170</v>
+      </c>
+      <c r="I8">
+        <f>F8/8760</f>
+        <v>0.19501559999999998</v>
+      </c>
+      <c r="J8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10">
+        <f>133815/1000</f>
+        <v>133.815</v>
+      </c>
+      <c r="C10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10">
+        <f>B10/I8</f>
+        <v>686.17587516075639</v>
+      </c>
+      <c r="E10" t="s">
+        <v>173</v>
+      </c>
+      <c r="F10">
+        <f>D10*I1</f>
+        <v>754.79346267683206</v>
+      </c>
+      <c r="G10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="M13" t="s">
+        <v>201</v>
+      </c>
+      <c r="N13" t="s">
+        <v>191</v>
+      </c>
+      <c r="O13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14">
+        <f>61753*1000</f>
+        <v>61753000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>180</v>
+      </c>
+      <c r="H14">
+        <f>B14/(D14*1000)</f>
+        <v>3087.65</v>
+      </c>
+      <c r="I14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14">
+        <f>B14/(D14*1000)</f>
+        <v>3087.65</v>
+      </c>
+      <c r="K14" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14">
+        <f>F8/J15</f>
+        <v>7.7067866558804763</v>
+      </c>
+      <c r="N14">
+        <f>F8/(J15+J14)</f>
+        <v>0.5162203858341059</v>
+      </c>
+      <c r="O14">
+        <f>J15/J14</f>
+        <v>7.1791339714719973E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15">
+        <v>1064000</v>
+      </c>
+      <c r="C15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>180</v>
+      </c>
+      <c r="H15" s="2">
+        <f>B15/(D15*1000)</f>
+        <v>35.466666666666669</v>
+      </c>
+      <c r="I15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="2">
+        <f>H15+F16</f>
+        <v>221.66653007015515</v>
+      </c>
+      <c r="K15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>212</v>
+      </c>
+      <c r="F16">
+        <v>186.19986340348848</v>
+      </c>
+      <c r="G16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17">
+        <v>1089000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17">
+        <f>B17/1000000</f>
+        <v>1.089</v>
+      </c>
+      <c r="E17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <f>B19*(365*24*60*60)</f>
+        <v>378432000</v>
+      </c>
+      <c r="C20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <f>B20*0.3</f>
+        <v>113529600</v>
+      </c>
+      <c r="C21" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21">
+        <f>B21*G1/(1000000)</f>
+        <v>1.0320872727272727</v>
+      </c>
+      <c r="E21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F21">
+        <f>D21/I1</f>
+        <v>0.93826115702479329</v>
+      </c>
+      <c r="G21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B23">
+        <f>(B14/1000000)+F21</f>
+        <v>62.69126115702479</v>
+      </c>
+      <c r="C23" t="s">
+        <v>184</v>
+      </c>
+      <c r="D23">
+        <f>B23*I1</f>
+        <v>68.960387272727274</v>
+      </c>
+      <c r="E23" t="s">
+        <v>182</v>
+      </c>
+      <c r="F23">
+        <f>D23/F8</f>
+        <v>4.0366977451736702E-2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26">
+        <f>D17</f>
+        <v>1.089</v>
+      </c>
+      <c r="C26" t="s">
+        <v>184</v>
+      </c>
+      <c r="D26">
+        <f>B26*I1</f>
+        <v>1.1979</v>
+      </c>
+      <c r="E26" t="s">
+        <v>182</v>
+      </c>
+      <c r="F26">
+        <f>D26/I8</f>
+        <v>6.1425855162356244</v>
+      </c>
+      <c r="G26" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="15"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B29">
+        <f>F8*B11*1000</f>
+        <v>34166733.119999997</v>
+      </c>
+      <c r="C29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B30">
+        <f>(B10*1000000)+(70005000*B11)</f>
+        <v>1533915000</v>
+      </c>
+      <c r="C30" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31">
+        <f>B30/B29</f>
+        <v>44.894985851079227</v>
+      </c>
+      <c r="C31" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33">
+        <v>1.3300000000000001E-4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <f>B33*F8</f>
+        <v>0.22720877524800001</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B35">
+        <v>14.95</v>
+      </c>
+      <c r="C35" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <f>B35*I1/1000</f>
+        <v>1.6445000000000001E-2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>211</v>
+      </c>
+      <c r="B37">
+        <v>2950</v>
+      </c>
+      <c r="C37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37">
+        <f>B37*C2</f>
+        <v>819.51</v>
+      </c>
+      <c r="E37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <f>D37*B34</f>
+        <v>186.19986340348848</v>
+      </c>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CD823C-69C1-4E4C-92FB-4F8D7DC530BE}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="M1" sqref="M1:N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -3186,8 +3733,14 @@
       <c r="K1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M1" s="10">
+        <v>0.27779999999999999</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2">
         <f>1/110</f>
         <v>9.0909090909090905E-3</v>
@@ -3202,7 +3755,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -3227,7 +3780,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>203</v>
       </c>
@@ -3252,7 +3805,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>181</v>
       </c>
@@ -3272,7 +3825,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9">
         <f>B8*(365*24*60*60)</f>
         <v>6937920</v>
@@ -3295,7 +3848,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10">
         <f>0.3*B9</f>
         <v>2081376</v>
@@ -3325,7 +3878,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F11">
         <f>F10*1000000</f>
         <v>17201.454545454544</v>
@@ -3334,7 +3887,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>206</v>
       </c>
@@ -3346,7 +3899,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>176</v>
       </c>
@@ -3364,7 +3917,7 @@
         <v>0.6410769230769231</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>204</v>
       </c>
@@ -3382,12 +3935,12 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>192</v>
       </c>
@@ -3399,7 +3952,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>195</v>
       </c>
@@ -3408,7 +3961,7 @@
         <v>3618029.0909090908</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>197</v>
       </c>

</xml_diff>

<commit_message>
updated CCS, steam reforming data
Former-commit-id: 9317fa3749951c39e37a26bdabcfe63dce1977e5
Former-commit-id: 869d51b68e403b7dff7af169a5bce93258cc0334
</commit_message>
<xml_diff>
--- a/data/i2cner-tech-data.xlsx
+++ b/data/i2cner-tech-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F730DAAD-5F76-409C-A4C2-30821CBECAAB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD86F2AE-1E36-47A8-A619-6179D077983E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="216">
   <si>
     <t>H2 Method</t>
   </si>
@@ -681,6 +681,12 @@
   </si>
   <si>
     <t>Total /yr</t>
+  </si>
+  <si>
+    <t>CCS Efficiency</t>
+  </si>
+  <si>
+    <t>Captured CO2</t>
   </si>
 </sst>
 </file>
@@ -3160,10 +3166,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AA85B1-F75D-401E-9CDA-9DC2F24930C6}">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3270,416 +3276,428 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>207</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>0.65</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>168</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>2.5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>169</v>
       </c>
-      <c r="D8">
-        <f>B8*(365*24*60*60)</f>
+      <c r="D9">
+        <f>B9*(365*24*60*60)</f>
         <v>78840000</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>116</v>
       </c>
-      <c r="F8">
-        <f>(D8*I3*C6/(1000000))</f>
+      <c r="F9">
+        <f>(D9*I3*C7/(1000000))</f>
         <v>1708.3366559999999</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>170</v>
       </c>
-      <c r="I8">
-        <f>F8/8760</f>
+      <c r="I9">
+        <f>F9/8760</f>
         <v>0.19501559999999998</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <f>133815/1000</f>
         <v>133.815</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>172</v>
       </c>
-      <c r="D10">
-        <f>B10/I8</f>
+      <c r="D11">
+        <f>B11/I9</f>
         <v>686.17587516075639</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>173</v>
       </c>
-      <c r="F10">
-        <f>D10*I1</f>
+      <c r="F11">
+        <f>D11*I1</f>
         <v>754.79346267683206</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M14" t="s">
         <v>201</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N14" t="s">
         <v>191</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O14" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>175</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <f>61753*1000</f>
         <v>61753000</v>
       </c>
-      <c r="C14" t="s">
-        <v>178</v>
-      </c>
-      <c r="D14">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>180</v>
-      </c>
-      <c r="H14">
-        <f>B14/(D14*1000)</f>
-        <v>3087.65</v>
-      </c>
-      <c r="I14" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14">
-        <f>B14/(D14*1000)</f>
-        <v>3087.65</v>
-      </c>
-      <c r="K14" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14">
-        <f>F8/J15</f>
-        <v>7.7067866558804763</v>
-      </c>
-      <c r="N14">
-        <f>F8/(J15+J14)</f>
-        <v>0.5162203858341059</v>
-      </c>
-      <c r="O14">
-        <f>J15/J14</f>
-        <v>7.1791339714719973E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>176</v>
-      </c>
-      <c r="B15">
-        <v>1064000</v>
-      </c>
       <c r="C15" t="s">
         <v>178</v>
       </c>
       <c r="D15">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
         <v>180</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15">
         <f>B15/(D15*1000)</f>
-        <v>35.466666666666669</v>
+        <v>3087.65</v>
       </c>
       <c r="I15" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="2">
-        <f>H15+F16</f>
-        <v>221.66653007015515</v>
+      <c r="J15">
+        <f>B15/(D15*1000)</f>
+        <v>3087.65</v>
       </c>
       <c r="K15" t="s">
         <v>35</v>
       </c>
+      <c r="M15">
+        <f>F9/J16</f>
+        <v>8.4135224595267211</v>
+      </c>
+      <c r="N15">
+        <f>F9/(J16+J15)</f>
+        <v>0.51914135299261088</v>
+      </c>
+      <c r="O15">
+        <f>J16/J15</f>
+        <v>6.5760867886517679E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>212</v>
-      </c>
-      <c r="F16">
-        <v>186.19986340348848</v>
-      </c>
-      <c r="G16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16">
+        <v>1064000</v>
+      </c>
+      <c r="C16" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>180</v>
+      </c>
+      <c r="H16" s="2">
+        <f>B16/(D16*1000)</f>
+        <v>35.466666666666669</v>
+      </c>
+      <c r="I16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="2">
+        <f>H16+F17</f>
+        <v>203.0465437298063</v>
+      </c>
+      <c r="K16" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>212</v>
+      </c>
+      <c r="F17">
+        <f>B39</f>
+        <v>167.57987706313963</v>
+      </c>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>177</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>1089000</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>178</v>
       </c>
-      <c r="D17">
-        <f>B17/1000000</f>
+      <c r="D18">
+        <f>B18/1000000</f>
         <v>1.089</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>181</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>12</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B20">
-        <f>B19*(365*24*60*60)</f>
-        <v>378432000</v>
-      </c>
-      <c r="C20" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21">
-        <f>B20*0.3</f>
+        <f>B20*(365*24*60*60)</f>
+        <v>378432000</v>
+      </c>
+      <c r="C21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <f>B21*0.3</f>
         <v>113529600</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>147</v>
       </c>
-      <c r="D21">
-        <f>B21*G1/(1000000)</f>
+      <c r="D22">
+        <f>B22*G1/(1000000)</f>
         <v>1.0320872727272727</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>182</v>
       </c>
-      <c r="F21">
-        <f>D21/I1</f>
+      <c r="F22">
+        <f>D22/I1</f>
         <v>0.93826115702479329</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G22" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B23">
-        <f>(B14/1000000)+F21</f>
+      <c r="B24">
+        <f>(B15/1000000)+F22</f>
         <v>62.69126115702479</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>184</v>
       </c>
-      <c r="D23">
-        <f>B23*I1</f>
+      <c r="D24">
+        <f>B24*I1</f>
         <v>68.960387272727274</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>182</v>
       </c>
-      <c r="F23">
-        <f>D23/F8</f>
+      <c r="F24">
+        <f>D24/F9</f>
         <v>4.0366977451736702E-2</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B26">
-        <f>D17</f>
+      <c r="B27">
+        <f>D18</f>
         <v>1.089</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>184</v>
       </c>
-      <c r="D26">
-        <f>B26*I1</f>
+      <c r="D27">
+        <f>B27*I1</f>
         <v>1.1979</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>182</v>
       </c>
-      <c r="F26">
-        <f>D26/I8</f>
+      <c r="F27">
+        <f>D27/I9</f>
         <v>6.1425855162356244</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B29">
-        <f>F8*B11*1000</f>
-        <v>34166733.119999997</v>
-      </c>
-      <c r="C29" t="s">
-        <v>194</v>
-      </c>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B30">
-        <f>(B10*1000000)+(70005000*B11)</f>
-        <v>1533915000</v>
+        <f>F9*B12*1000</f>
+        <v>34166733.119999997</v>
       </c>
       <c r="C30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B31">
+        <f>(B11*1000000)+(70005000*B12)</f>
+        <v>1533915000</v>
+      </c>
+      <c r="C31" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B31">
-        <f>B30/B29</f>
+      <c r="B32">
+        <f>B31/B30</f>
         <v>44.894985851079227</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>1.3300000000000001E-4</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B34">
-        <f>B33*F8</f>
-        <v>0.22720877524800001</v>
-      </c>
-      <c r="C34" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B35">
+        <f>B34*F9*B5</f>
+        <v>0.2044878977232</v>
+      </c>
+      <c r="C35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="15" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>14.95</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B36">
-        <f>B35*I1/1000</f>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <f>B36*I1/1000</f>
         <v>1.6445000000000001E-2</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>211</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>2950</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>51</v>
       </c>
-      <c r="D37">
-        <f>B37*C2</f>
+      <c r="D38">
+        <f>B38*C2</f>
         <v>819.51</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B38">
-        <f>D37*B34</f>
-        <v>186.19986340348848</v>
-      </c>
-      <c r="C38" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="3">
+        <f>D38*B35</f>
+        <v>167.57987706313963</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added novel tech model, reorganized active model
Former-commit-id: 4fc743e9ce634f59cb1472e094bc0bd7a5236ab4
Former-commit-id: 52e5324765ebbbd277157aa00b6c496cfd9b7f3e
</commit_message>
<xml_diff>
--- a/data/i2cner-tech-data.xlsx
+++ b/data/i2cner-tech-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD86F2AE-1E36-47A8-A619-6179D077983E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F192ABA5-BCB4-4D15-A6A9-C8189946C44B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
+    <workbookView xWindow="25995" yWindow="3600" windowWidth="21600" windowHeight="11325" firstSheet="5" activeTab="8" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CCS" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="219">
   <si>
     <t>H2 Method</t>
   </si>
@@ -599,9 +599,6 @@
     <t>FixedOM</t>
   </si>
   <si>
-    <t>Total(w/o ELC)</t>
-  </si>
-  <si>
     <t>GW</t>
   </si>
   <si>
@@ -687,6 +684,18 @@
   </si>
   <si>
     <t>Captured CO2</t>
+  </si>
+  <si>
+    <t>VAROM(w/o ELC)</t>
+  </si>
+  <si>
+    <t>other OM</t>
+  </si>
+  <si>
+    <t>Difference(CCS)</t>
+  </si>
+  <si>
+    <t>water+fuel+CCS material</t>
   </si>
 </sst>
 </file>
@@ -770,7 +779,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -780,6 +789,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -812,7 +827,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -836,6 +851,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2733,12 +2749,12 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="A1:XFD1048576"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
@@ -2839,13 +2855,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C6">
         <v>0.65</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -2877,7 +2893,7 @@
         <v>0.19501559999999998</v>
       </c>
       <c r="J8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2898,12 +2914,12 @@
       <c r="E10" t="s">
         <v>173</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="17">
         <f>D10*I1</f>
         <v>754.79346267683206</v>
       </c>
       <c r="G10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2914,7 +2930,7 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2925,16 +2941,16 @@
         <v>179</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="I13" t="s">
         <v>189</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>190</v>
       </c>
-      <c r="J13" t="s">
-        <v>191</v>
-      </c>
       <c r="K13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2969,7 +2985,7 @@
         <f>F8/(F15+F14)</f>
         <v>0.54699738701190581</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="17">
         <f>F15/F14</f>
         <v>1.1486621432696928E-2</v>
       </c>
@@ -3064,7 +3080,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="B23">
         <f>(B14/1000000)+F21</f>
@@ -3080,7 +3096,7 @@
       <c r="E23" t="s">
         <v>182</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="17">
         <f>D23/F8</f>
         <v>4.0366977451736702E-2</v>
       </c>
@@ -3090,7 +3106,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -3111,44 +3127,46 @@
       <c r="E26" t="s">
         <v>182</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="17">
         <f>D26/I8</f>
         <v>6.1425855162356244</v>
       </c>
       <c r="G26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
+      <c r="A27" s="15" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B29">
         <f>F8*B11*1000</f>
         <v>34166733.119999997</v>
       </c>
       <c r="C29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B30">
         <f>(B10*1000000)+(70005000*B11)</f>
         <v>1533915000</v>
       </c>
       <c r="C30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B31">
         <f>B30/B29</f>
@@ -3166,10 +3184,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AA85B1-F75D-401E-9CDA-9DC2F24930C6}">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3186,7 +3204,7 @@
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C1" s="5">
         <v>41.869</v>
       </c>
@@ -3210,7 +3228,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="10">
@@ -3226,7 +3244,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3258,7 +3276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -3276,26 +3294,26 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B5">
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7">
+        <v>0.7</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="C7">
-        <v>0.65</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>168</v>
       </c>
@@ -3314,46 +3332,45 @@
       </c>
       <c r="F9">
         <f>(D9*I3*C7/(1000000))</f>
-        <v>1708.3366559999999</v>
+        <v>1839.7471680000001</v>
       </c>
       <c r="G9" t="s">
         <v>170</v>
       </c>
       <c r="I9">
         <f>F9/8760</f>
-        <v>0.19501559999999998</v>
+        <v>0.2100168</v>
       </c>
       <c r="J9" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>171</v>
       </c>
       <c r="B11">
-        <f>133815/1000</f>
-        <v>133.815</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
         <v>172</v>
       </c>
       <c r="D11">
         <f>B11/I9</f>
-        <v>686.17587516075639</v>
+        <v>771.36686207960508</v>
       </c>
       <c r="E11" t="s">
         <v>173</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="17">
         <f>D11*I1</f>
-        <v>754.79346267683206</v>
+        <v>848.50354828756565</v>
       </c>
       <c r="G11" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>68</v>
       </c>
@@ -3361,10 +3378,10 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>174</v>
       </c>
@@ -3372,28 +3389,19 @@
         <v>179</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="M14" t="s">
-        <v>201</v>
-      </c>
-      <c r="N14" t="s">
-        <v>191</v>
-      </c>
-      <c r="O14" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>175</v>
       </c>
       <c r="B15">
-        <f>61753*1000</f>
-        <v>61753000</v>
+        <f>64546*1000</f>
+        <v>64546000</v>
       </c>
       <c r="C15" t="s">
         <v>178</v>
@@ -3406,32 +3414,20 @@
       </c>
       <c r="H15">
         <f>B15/(D15*1000)</f>
-        <v>3087.65</v>
+        <v>3227.3</v>
       </c>
       <c r="I15" t="s">
         <v>35</v>
       </c>
       <c r="J15">
         <f>B15/(D15*1000)</f>
-        <v>3087.65</v>
+        <v>3227.3</v>
       </c>
       <c r="K15" t="s">
         <v>35</v>
       </c>
-      <c r="M15">
-        <f>F9/J16</f>
-        <v>8.4135224595267211</v>
-      </c>
-      <c r="N15">
-        <f>F9/(J16+J15)</f>
-        <v>0.51914135299261088</v>
-      </c>
-      <c r="O15">
-        <f>J16/J15</f>
-        <v>6.5760867886517679E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>176</v>
       </c>
@@ -3456,25 +3452,25 @@
       </c>
       <c r="J16" s="2">
         <f>H16+F17</f>
-        <v>203.0465437298063</v>
+        <v>215.93730350389399</v>
       </c>
       <c r="K16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F17">
-        <f>B39</f>
-        <v>167.57987706313963</v>
+        <f>B40</f>
+        <v>180.47063683722732</v>
       </c>
       <c r="G17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>177</v>
       </c>
@@ -3492,212 +3488,254 @@
         <v>184</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B19">
+        <f>(97662-64546-2778-1064-1089)*1000</f>
+        <v>28185000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>178</v>
+      </c>
+      <c r="H19" t="s">
+        <v>200</v>
+      </c>
+      <c r="I19" t="s">
+        <v>190</v>
+      </c>
+      <c r="J19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <f>F9/J16</f>
+        <v>8.5198209764938735</v>
+      </c>
+      <c r="I20">
+        <f>F9/(J16+J15)</f>
+        <v>0.53430739906536318</v>
+      </c>
+      <c r="J20" s="17">
+        <f>J16/J15</f>
+        <v>6.6909584948376039E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>181</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>12</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21">
-        <f>B20*(365*24*60*60)</f>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <f>B21*(365*24*60*60)</f>
         <v>378432000</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <f>B21*0.3</f>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <f>B22*0.3</f>
         <v>113529600</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>147</v>
       </c>
-      <c r="D22">
-        <f>B22*G1/(1000000)</f>
+      <c r="D23">
+        <f>B23*G1/(1000000)</f>
         <v>1.0320872727272727</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>182</v>
       </c>
-      <c r="F22">
-        <f>D22/I1</f>
+      <c r="F23">
+        <f>D23/I1</f>
         <v>0.93826115702479329</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B24">
-        <f>(B15/1000000)+F22</f>
-        <v>62.69126115702479</v>
-      </c>
-      <c r="C24" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25">
+        <f>(B15/1000000)+F23</f>
+        <v>65.484261157024804</v>
+      </c>
+      <c r="C25" t="s">
         <v>184</v>
       </c>
-      <c r="D24">
-        <f>B24*I1</f>
-        <v>68.960387272727274</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D25">
+        <f>B25*I1</f>
+        <v>72.032687272727287</v>
+      </c>
+      <c r="E25" t="s">
         <v>182</v>
       </c>
-      <c r="F24">
-        <f>D24/F9</f>
-        <v>4.0366977451736702E-2</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="F25" s="17">
+        <f>(D25/F9)+B38</f>
+        <v>5.5653579647052503E-2</v>
+      </c>
+      <c r="G25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <f>D18</f>
         <v>1.089</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>184</v>
       </c>
-      <c r="D27">
-        <f>B27*I1</f>
+      <c r="D28">
+        <f>B28*I1</f>
         <v>1.1979</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>182</v>
       </c>
-      <c r="F27">
-        <f>D27/I9</f>
-        <v>6.1425855162356244</v>
-      </c>
-      <c r="G27" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B30">
+      <c r="F28" s="17">
+        <f>D28/I9</f>
+        <v>5.7038294079330791</v>
+      </c>
+      <c r="G28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B31">
         <f>F9*B12*1000</f>
-        <v>34166733.119999997</v>
-      </c>
-      <c r="C30" t="s">
+        <v>36794943.360000007</v>
+      </c>
+      <c r="C31" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="B32">
+        <f>(B11*1000000)+(97662000*B12)</f>
+        <v>2115240000</v>
+      </c>
+      <c r="C32" t="s">
         <v>195</v>
       </c>
-      <c r="B31">
-        <f>(B11*1000000)+(70005000*B12)</f>
-        <v>1533915000</v>
-      </c>
-      <c r="C31" t="s">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B32">
-        <f>B31/B30</f>
-        <v>44.894985851079227</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B33">
+        <f>B32/B31</f>
+        <v>57.487247073723978</v>
+      </c>
+      <c r="C33" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>1.3300000000000001E-4</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B35">
-        <f>B34*F9*B5</f>
-        <v>0.2044878977232</v>
-      </c>
-      <c r="C35" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B36">
+        <f>B35*F9*B5</f>
+        <v>0.22021773600960004</v>
+      </c>
+      <c r="C36" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="15" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B37">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
         <v>209</v>
       </c>
-      <c r="B36">
-        <v>14.95</v>
-      </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="17">
+        <f>B37*I1/1000</f>
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38">
+        <f>B38*F9*1000000/I1</f>
+        <v>27596207.52</v>
+      </c>
+      <c r="F38" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B37">
-        <f>B36*I1/1000</f>
-        <v>1.6445000000000001E-2</v>
-      </c>
-      <c r="C37" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>211</v>
-      </c>
-      <c r="B38">
+      <c r="B39">
         <v>2950</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>51</v>
       </c>
-      <c r="D38">
-        <f>B38*C2</f>
+      <c r="D39">
+        <f>B39*C2</f>
         <v>819.51</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="3">
-        <f>D38*B35</f>
-        <v>167.57987706313963</v>
-      </c>
-      <c r="C39" s="3" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="3">
+        <f>D39*B36</f>
+        <v>180.47063683722732</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3711,7 +3749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CD823C-69C1-4E4C-92FB-4F8D7DC530BE}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M1" sqref="M1:N1"/>
     </sheetView>
   </sheetViews>
@@ -3781,7 +3819,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
         <v>171</v>
@@ -3800,13 +3838,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B6">
         <v>2974000</v>
       </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D6">
         <f>B6/(1000000*L10)</f>
@@ -3820,7 +3858,7 @@
         <v>1362.9742953897025</v>
       </c>
       <c r="G6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -3834,7 +3872,7 @@
         <v>169</v>
       </c>
       <c r="I8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J8">
         <v>0.02</v>
@@ -3893,7 +3931,7 @@
         <v>2.4001919999999998E-3</v>
       </c>
       <c r="M10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -3907,7 +3945,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B12">
         <f>D10/L9</f>
@@ -3928,7 +3966,7 @@
         <v>124</v>
       </c>
       <c r="I14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J14">
         <f>J1/B14</f>
@@ -3937,7 +3975,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B16">
         <v>15000</v>
@@ -3950,29 +3988,29 @@
         <v>6.8744500439964815</v>
       </c>
       <c r="E16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B19">
         <f>L9*B4/1000</f>
         <v>0.42051363839999994</v>
       </c>
       <c r="C19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B20">
         <f>B6+(B16*B4)+(F11*B4)</f>
@@ -3981,7 +4019,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B21">
         <f>B20/B19</f>

</xml_diff>

<commit_message>
added ccs reservoir trends
Former-commit-id: 262bf8ff5acd222d8ff4c3f4d4b32f09c707ecfc
Former-commit-id: 709aa697acd0578bda943a73cac47237ec25f2e5
</commit_message>
<xml_diff>
--- a/data/i2cner-tech-data.xlsx
+++ b/data/i2cner-tech-data.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0D1D17-3A33-4C12-9C9A-3DE787AD042E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006B096D-F042-435E-869B-F93B49E7F92D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33165" yWindow="3345" windowWidth="13830" windowHeight="7170" firstSheet="4" activeTab="10" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
+    <workbookView xWindow="32895" yWindow="4095" windowWidth="21600" windowHeight="11325" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CCS" sheetId="2" r:id="rId1"/>
-    <sheet name="JHFC" sheetId="1" r:id="rId2"/>
-    <sheet name="Acar and Dincer" sheetId="6" r:id="rId3"/>
-    <sheet name="H2 Steam Reforming" sheetId="3" r:id="rId4"/>
-    <sheet name="Photocatalytic H2" sheetId="4" r:id="rId5"/>
-    <sheet name="Kato_H2" sheetId="7" r:id="rId6"/>
-    <sheet name="Keipi_SMR" sheetId="5" r:id="rId7"/>
-    <sheet name="KEIPI_CCSSMR" sheetId="9" r:id="rId8"/>
-    <sheet name="Keipi_electrolysis" sheetId="8" r:id="rId9"/>
-    <sheet name="Simons_PEMFC" sheetId="10" r:id="rId10"/>
-    <sheet name="EIA_LCOE" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId2"/>
+    <sheet name="JHFC" sheetId="1" r:id="rId3"/>
+    <sheet name="Acar and Dincer" sheetId="6" r:id="rId4"/>
+    <sheet name="H2 Steam Reforming" sheetId="3" r:id="rId5"/>
+    <sheet name="Photocatalytic H2" sheetId="4" r:id="rId6"/>
+    <sheet name="Kato_H2" sheetId="7" r:id="rId7"/>
+    <sheet name="Keipi_SMR" sheetId="5" r:id="rId8"/>
+    <sheet name="KEIPI_CCSSMR" sheetId="9" r:id="rId9"/>
+    <sheet name="Keipi_electrolysis" sheetId="8" r:id="rId10"/>
+    <sheet name="Simons_PEMFC" sheetId="10" r:id="rId11"/>
+    <sheet name="EIA_LCOE" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="247">
   <si>
     <t>H2 Method</t>
   </si>
@@ -764,14 +765,33 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>CCS Trend</t>
+  </si>
+  <si>
+    <t>example: Hadi</t>
+  </si>
+  <si>
+    <t>fraction</t>
+  </si>
+  <si>
+    <t>Total(Mt)</t>
+  </si>
+  <si>
+    <t>Value(Mt)</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.00000000E+00"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -907,7 +927,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -929,14 +949,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1258,10 +1279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C7BE1D-16BA-4023-AA64-49E118FA5EEE}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8:N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1270,6 +1291,7 @@
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" customWidth="1"/>
     <col min="12" max="12" width="10.6640625" customWidth="1"/>
@@ -1692,6 +1714,125 @@
         <v>18</v>
       </c>
     </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>242</v>
+      </c>
+      <c r="B29">
+        <v>2020</v>
+      </c>
+      <c r="C29">
+        <v>2E-3</v>
+      </c>
+      <c r="D29">
+        <v>100</v>
+      </c>
+      <c r="E29">
+        <f>C29*$D$29</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>2025</v>
+      </c>
+      <c r="C30">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ref="E30:E36" si="4">C30*$D$29</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>2030</v>
+      </c>
+      <c r="C31">
+        <v>0.02</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>2035</v>
+      </c>
+      <c r="C32">
+        <v>0.06</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>2040</v>
+      </c>
+      <c r="C33">
+        <v>0.2</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>2045</v>
+      </c>
+      <c r="C34">
+        <v>0.5</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>2050</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>2100</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="4"/>
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1699,6 +1840,354 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CD823C-69C1-4E4C-92FB-4F8D7DC530BE}">
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1">
+        <v>5024.28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1">
+        <v>1395.7449839999999</v>
+      </c>
+      <c r="I1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1">
+        <v>33.335999999999999</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="10">
+        <v>0.27779999999999999</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <f>1/110</f>
+        <v>9.0909090909090905E-3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <f>3.9</f>
+        <v>3.9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>236</v>
+      </c>
+      <c r="J3">
+        <f>J1-J2</f>
+        <v>29.436</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4">
+        <f>1000*D2</f>
+        <v>1100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4">
+        <f>600*D2</f>
+        <v>660</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6">
+        <v>2974000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D6">
+        <f>B6/(1000000*L10)</f>
+        <v>1239.0675412633659</v>
+      </c>
+      <c r="E6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F6">
+        <f>D6*D2</f>
+        <v>1362.9742953897025</v>
+      </c>
+      <c r="G6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8">
+        <v>0.22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>169</v>
+      </c>
+      <c r="I8" t="s">
+        <v>198</v>
+      </c>
+      <c r="J8">
+        <v>0.02</v>
+      </c>
+      <c r="K8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <f>B8*(365*24*60*60)</f>
+        <v>6937920</v>
+      </c>
+      <c r="C9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9">
+        <f>J8*(365*24*60*60)</f>
+        <v>630720</v>
+      </c>
+      <c r="K9" t="s">
+        <v>116</v>
+      </c>
+      <c r="L9">
+        <f>J9*J1/1000000</f>
+        <v>21.025681919999997</v>
+      </c>
+      <c r="M9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <f>0.3*B9</f>
+        <v>2081376</v>
+      </c>
+      <c r="C10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10">
+        <f>B10*B2/1000000</f>
+        <v>1.89216E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>182</v>
+      </c>
+      <c r="F10">
+        <f>D10/D2</f>
+        <v>1.7201454545454544E-2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>184</v>
+      </c>
+      <c r="L10">
+        <f>L9/8760</f>
+        <v>2.4001919999999998E-3</v>
+      </c>
+      <c r="M10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <f>F10*1000000</f>
+        <v>17201.454545454544</v>
+      </c>
+      <c r="G11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B12">
+        <f>D10/L9</f>
+        <v>8.9992800575953936E-4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>124</v>
+      </c>
+      <c r="I14" t="s">
+        <v>200</v>
+      </c>
+      <c r="J14">
+        <f>J1/B14</f>
+        <v>0.6410769230769231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16">
+        <v>15000</v>
+      </c>
+      <c r="C16" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16">
+        <f>B16*D2/(1000000*L10)</f>
+        <v>6.8744500439964815</v>
+      </c>
+      <c r="E16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B19">
+        <f>L9*B4/1000</f>
+        <v>0.42051363839999994</v>
+      </c>
+      <c r="C19" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B20">
+        <f>B6+(B16*B4)+(F11*B4)</f>
+        <v>3618029.0909090908</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B21">
+        <f>B20/B19</f>
+        <v>8603832.9331605602</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24">
+        <v>2017</v>
+      </c>
+      <c r="C24">
+        <v>1160</v>
+      </c>
+      <c r="D24" t="s">
+        <v>235</v>
+      </c>
+      <c r="E24">
+        <f>C24/J3</f>
+        <v>39.407528196765867</v>
+      </c>
+      <c r="F24" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>2050</v>
+      </c>
+      <c r="C25">
+        <v>480</v>
+      </c>
+      <c r="D25" t="s">
+        <v>235</v>
+      </c>
+      <c r="E25">
+        <f>C25/J3</f>
+        <v>16.306563391765184</v>
+      </c>
+      <c r="F25" t="s">
+        <v>224</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8767C190-EC74-43BE-8FB1-1D4B5E66E226}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -1781,7 +2270,7 @@
         <f>F4/1000000</f>
         <v>3.424657534246575E-7</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="17">
         <f>942/1000000</f>
         <v>9.4200000000000002E-4</v>
       </c>
@@ -1792,11 +2281,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23AAF198-3247-41A0-820F-167859A4EE2B}">
   <dimension ref="A3:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -1809,19 +2298,19 @@
       <c r="B3" s="2">
         <v>2017</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="19">
         <v>2025</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21">
+      <c r="D3" s="19"/>
+      <c r="E3" s="22">
         <v>2040</v>
       </c>
-      <c r="F3" s="21"/>
+      <c r="F3" s="22"/>
       <c r="G3" t="s">
         <v>234</v>
       </c>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -1839,8 +2328,8 @@
       <c r="F4" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1868,8 +2357,8 @@
         <f>E5/C5</f>
         <v>0.83100167879127029</v>
       </c>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1897,8 +2386,8 @@
         <f>E6/C6</f>
         <v>0.9003754693366709</v>
       </c>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1926,7 +2415,7 @@
         <f>E7/C7</f>
         <v>0.69963190184049073</v>
       </c>
-      <c r="R7" s="19"/>
+      <c r="R7" s="18"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -2065,6 +2554,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E6C6BEB-6091-4743-A766-86BDD24D0263}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47851EB-8A83-4629-AF5F-F0859B72869A}">
   <dimension ref="A2:P30"/>
   <sheetViews>
@@ -2258,10 +2759,10 @@
       <c r="G10" t="s">
         <v>139</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="K10" s="17"/>
+      <c r="K10" s="21"/>
       <c r="L10" s="12">
         <f>L9/G5</f>
         <v>122583.35123523093</v>
@@ -2271,10 +2772,10 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="K11" s="17"/>
+      <c r="K11" s="21"/>
       <c r="L11" s="12">
         <f>M4*L10</f>
         <v>4086438.5967776584</v>
@@ -2582,7 +3083,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F6EB48-4038-4170-8B3C-AD75DD5549D7}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2622,16 +3123,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26522F16-178D-4C9D-9097-E5B0FFBFDA90}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="5" width="17.44140625" customWidth="1"/>
     <col min="6" max="6" width="13.44140625" customWidth="1"/>
@@ -2640,8 +3142,7 @@
     <col min="10" max="11" width="13.33203125" customWidth="1"/>
     <col min="12" max="12" width="16.6640625" customWidth="1"/>
     <col min="14" max="14" width="15.33203125" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" customWidth="1"/>
+    <col min="15" max="16" width="16.33203125" customWidth="1"/>
     <col min="17" max="17" width="15.109375" customWidth="1"/>
     <col min="18" max="18" width="11" customWidth="1"/>
   </cols>
@@ -2846,7 +3347,7 @@
       <c r="N6" t="s">
         <v>78</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="20">
         <f>87/(1000000*0.27777)</f>
         <v>3.1320876984555567E-4</v>
       </c>
@@ -3017,7 +3518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D8D9EFC-D052-4551-86BD-609CA1895FF2}">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -3095,7 +3596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E890F7-EE40-41D8-8D6F-926E6C8520D6}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -3201,7 +3702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5DFEF8-915B-4056-B382-3EF1CD6D8429}">
   <dimension ref="A1:K31"/>
   <sheetViews>
@@ -3645,7 +4146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AA85B1-F75D-401E-9CDA-9DC2F24930C6}">
   <dimension ref="A1:K40"/>
   <sheetViews>
@@ -4206,352 +4707,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CD823C-69C1-4E4C-92FB-4F8D7DC530BE}">
-  <dimension ref="A1:N25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>120</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1">
-        <v>5024.28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H1">
-        <v>1395.7449839999999</v>
-      </c>
-      <c r="I1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J1">
-        <v>33.335999999999999</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="10">
-        <v>0.27779999999999999</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B2">
-        <f>1/110</f>
-        <v>9.0909090909090905E-3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E2" t="s">
-        <v>183</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2">
-        <f>3.9</f>
-        <v>3.9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="I3" t="s">
-        <v>236</v>
-      </c>
-      <c r="J3">
-        <f>J1-J2</f>
-        <v>29.436</v>
-      </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E4">
-        <f>1000*D2</f>
-        <v>1100</v>
-      </c>
-      <c r="F4" t="s">
-        <v>139</v>
-      </c>
-      <c r="G4">
-        <f>600*D2</f>
-        <v>660</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6">
-        <v>2974000</v>
-      </c>
-      <c r="C6" t="s">
-        <v>195</v>
-      </c>
-      <c r="D6">
-        <f>B6/(1000000*L10)</f>
-        <v>1239.0675412633659</v>
-      </c>
-      <c r="E6" t="s">
-        <v>173</v>
-      </c>
-      <c r="F6">
-        <f>D6*D2</f>
-        <v>1362.9742953897025</v>
-      </c>
-      <c r="G6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>181</v>
-      </c>
-      <c r="B8">
-        <v>0.22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>169</v>
-      </c>
-      <c r="I8" t="s">
-        <v>198</v>
-      </c>
-      <c r="J8">
-        <v>0.02</v>
-      </c>
-      <c r="K8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <f>B8*(365*24*60*60)</f>
-        <v>6937920</v>
-      </c>
-      <c r="C9" t="s">
-        <v>116</v>
-      </c>
-      <c r="J9">
-        <f>J8*(365*24*60*60)</f>
-        <v>630720</v>
-      </c>
-      <c r="K9" t="s">
-        <v>116</v>
-      </c>
-      <c r="L9">
-        <f>J9*J1/1000000</f>
-        <v>21.025681919999997</v>
-      </c>
-      <c r="M9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <f>0.3*B9</f>
-        <v>2081376</v>
-      </c>
-      <c r="C10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D10">
-        <f>B10*B2/1000000</f>
-        <v>1.89216E-2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>182</v>
-      </c>
-      <c r="F10">
-        <f>D10/D2</f>
-        <v>1.7201454545454544E-2</v>
-      </c>
-      <c r="G10" t="s">
-        <v>184</v>
-      </c>
-      <c r="L10">
-        <f>L9/8760</f>
-        <v>2.4001919999999998E-3</v>
-      </c>
-      <c r="M10" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F11">
-        <f>F10*1000000</f>
-        <v>17201.454545454544</v>
-      </c>
-      <c r="G11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B12">
-        <f>D10/L9</f>
-        <v>8.9992800575953936E-4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>176</v>
-      </c>
-      <c r="B14">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>124</v>
-      </c>
-      <c r="I14" t="s">
-        <v>200</v>
-      </c>
-      <c r="J14">
-        <f>J1/B14</f>
-        <v>0.6410769230769231</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B16">
-        <v>15000</v>
-      </c>
-      <c r="C16" t="s">
-        <v>178</v>
-      </c>
-      <c r="D16">
-        <f>B16*D2/(1000000*L10)</f>
-        <v>6.8744500439964815</v>
-      </c>
-      <c r="E16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B19">
-        <f>L9*B4/1000</f>
-        <v>0.42051363839999994</v>
-      </c>
-      <c r="C19" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B20">
-        <f>B6+(B16*B4)+(F11*B4)</f>
-        <v>3618029.0909090908</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B21">
-        <f>B20/B19</f>
-        <v>8603832.9331605602</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B24">
-        <v>2017</v>
-      </c>
-      <c r="C24">
-        <v>1160</v>
-      </c>
-      <c r="D24" t="s">
-        <v>235</v>
-      </c>
-      <c r="E24">
-        <f>C24/J3</f>
-        <v>39.407528196765867</v>
-      </c>
-      <c r="F24" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B25">
-        <v>2050</v>
-      </c>
-      <c r="C25">
-        <v>480</v>
-      </c>
-      <c r="D25" t="s">
-        <v>235</v>
-      </c>
-      <c r="E25">
-        <f>C25/J3</f>
-        <v>16.306563391765184</v>
-      </c>
-      <c r="F25" t="s">
-        <v>224</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated model capacity  values
Former-commit-id: 5885f6f353fce0af7e4d2c47086e8982252a00c0
Former-commit-id: beb6bab7a54a0428e29d6f1d4a30827720c71af7
</commit_message>
<xml_diff>
--- a/data/i2cner-tech-data.xlsx
+++ b/data/i2cner-tech-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FC18CE-A958-4B3C-AAFF-1F99E5852BF6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48FB379-1C6E-4F59-BBDC-19F34217ED84}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CCS_Costs_Early" sheetId="14" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="258">
   <si>
     <t>H2 Method</t>
   </si>
@@ -806,6 +806,18 @@
   </si>
   <si>
     <t>Cap Cost(MUSD/GWh)</t>
+  </si>
+  <si>
+    <t>H2 Cost</t>
+  </si>
+  <si>
+    <t>Total Generation</t>
+  </si>
+  <si>
+    <t>Annual Generation</t>
+  </si>
+  <si>
+    <t>Cap</t>
   </si>
 </sst>
 </file>
@@ -816,7 +828,7 @@
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="0.00000000E+00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -894,6 +906,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -950,7 +970,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -990,6 +1010,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1308,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3B25EB-4023-477D-80C4-74718858ACC8}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33:P44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2319,13 +2340,13 @@
         <v>239</v>
       </c>
       <c r="B31" s="20">
-        <v>495</v>
-      </c>
-      <c r="C31" s="20">
-        <v>4</v>
-      </c>
-      <c r="D31" s="20">
-        <v>2.6473008613171967E-2</v>
+        <v>764</v>
+      </c>
+      <c r="C31">
+        <v>6.214611477952583</v>
+      </c>
+      <c r="D31">
+        <v>4.084030751199931E-2</v>
       </c>
       <c r="E31">
         <v>0.7</v>
@@ -2346,7 +2367,7 @@
       </c>
       <c r="B32" s="2">
         <f>6*B31</f>
-        <v>2970</v>
+        <v>4584</v>
       </c>
       <c r="C32" s="21">
         <v>33</v>
@@ -2393,7 +2414,7 @@
       </c>
       <c r="P33" s="3">
         <f>$D$31+O33</f>
-        <v>6.3097008613171968E-2</v>
+        <v>7.7464307511999314E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
@@ -2422,7 +2443,7 @@
       </c>
       <c r="P34" s="3">
         <f t="shared" ref="P34:P44" si="17">$D$31+O34</f>
-        <v>7.0945008613171975E-2</v>
+        <v>8.5312307511999308E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
@@ -2458,7 +2479,7 @@
       </c>
       <c r="P35" s="3">
         <f t="shared" si="17"/>
-        <v>7.1468208613171977E-2</v>
+        <v>8.5835507511999309E-2</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -2494,7 +2515,7 @@
       </c>
       <c r="P36" s="3">
         <f t="shared" si="17"/>
-        <v>7.1991408613171978E-2</v>
+        <v>8.6358707511999311E-2</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
@@ -2530,7 +2551,7 @@
       </c>
       <c r="P37" s="3">
         <f t="shared" si="17"/>
-        <v>7.251460861317198E-2</v>
+        <v>8.6881907511999312E-2</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
@@ -2556,7 +2577,7 @@
       </c>
       <c r="P38" s="3">
         <f t="shared" si="17"/>
-        <v>7.3037808613171981E-2</v>
+        <v>8.7405107511999314E-2</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
@@ -2582,7 +2603,7 @@
       </c>
       <c r="P39" s="3">
         <f t="shared" si="17"/>
-        <v>7.3561008613171969E-2</v>
+        <v>8.7928307511999315E-2</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
@@ -2608,7 +2629,7 @@
       </c>
       <c r="P40" s="3">
         <f t="shared" si="17"/>
-        <v>7.408420861317197E-2</v>
+        <v>8.8451507511999317E-2</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -2634,7 +2655,7 @@
       </c>
       <c r="P41" s="3">
         <f t="shared" si="17"/>
-        <v>7.4607408613171985E-2</v>
+        <v>8.8974707511999318E-2</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
@@ -2660,7 +2681,7 @@
       </c>
       <c r="P42" s="3">
         <f t="shared" si="17"/>
-        <v>7.5130608613171973E-2</v>
+        <v>8.9497907511999319E-2</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -2686,7 +2707,7 @@
       </c>
       <c r="P43" s="3">
         <f t="shared" si="17"/>
-        <v>7.5653808613171974E-2</v>
+        <v>9.0021107511999321E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -2712,7 +2733,7 @@
       </c>
       <c r="P44" s="3">
         <f t="shared" si="17"/>
-        <v>7.6177008613171976E-2</v>
+        <v>9.0544307511999322E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4099,8 +4120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341C9435-D140-4ACE-89B8-673675A87D0E}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5110,7 +5131,7 @@
         <v>239</v>
       </c>
       <c r="B31" s="20">
-        <v>495</v>
+        <v>764</v>
       </c>
       <c r="C31" s="20">
         <v>4</v>
@@ -5137,7 +5158,7 @@
       </c>
       <c r="B32" s="2">
         <f>2*B31</f>
-        <v>990</v>
+        <v>1528</v>
       </c>
       <c r="C32" s="21">
         <v>4</v>
@@ -6719,10 +6740,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5DFEF8-915B-4056-B382-3EF1CD6D8429}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F38" sqref="F33:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6832,387 +6853,444 @@
         <v>88</v>
       </c>
     </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6">
+        <v>44.1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7">
+        <f>(133815+(B21*70004))*1000</f>
+        <v>2233935000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>158</v>
+      </c>
+    </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>255</v>
       </c>
       <c r="B8">
-        <v>2.5</v>
+        <f>B7/B6</f>
+        <v>50656122.448979594</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D8">
-        <f>B8*(365*24*60*60)</f>
-        <v>78840000</v>
-      </c>
-      <c r="E8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8">
-        <f>(D8*I3/(1000000))</f>
-        <v>2320.7342400000002</v>
-      </c>
-      <c r="G8" t="s">
-        <v>133</v>
-      </c>
-      <c r="I8">
-        <f>F8/8760</f>
-        <v>0.26492400000000005</v>
-      </c>
-      <c r="J8" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>256</v>
+      </c>
+      <c r="B9">
+        <f>B8/(B21*1000)</f>
+        <v>1688.5374149659865</v>
+      </c>
+      <c r="C9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B10">
+        <f>B9/8760</f>
+        <v>0.19275541266735005</v>
+      </c>
+      <c r="C10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12">
+        <v>2.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12">
+        <f>B12*(365*24*60*60)</f>
+        <v>78840000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12">
+        <v>1688.5374149659865</v>
+      </c>
+      <c r="G12" t="s">
+        <v>133</v>
+      </c>
+      <c r="I12">
+        <v>0.19275541266735</v>
+      </c>
+      <c r="J12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>225</v>
       </c>
-      <c r="B9">
+      <c r="B13">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C13" t="s">
         <v>132</v>
       </c>
-      <c r="D9">
-        <f>B9*B17*365*24*3600/1000000000</f>
+      <c r="D13">
+        <f>B13*B21*365*24*3600/1000000000</f>
         <v>22.705919999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B11">
+      <c r="B15">
         <f>133815/1000</f>
         <v>133.815</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C15" t="s">
         <v>135</v>
       </c>
-      <c r="D11">
-        <f>B11/I8</f>
-        <v>505.10712506228191</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D15">
+        <f>B15/I12</f>
+        <v>694.22175049855991</v>
+      </c>
+      <c r="E15" t="s">
         <v>136</v>
       </c>
-      <c r="F11" s="15">
-        <f>D11*I1</f>
-        <v>555.61783756851014</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F15" s="15">
+        <f>D15*I1</f>
+        <v>763.64392554841595</v>
+      </c>
+      <c r="G15" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="B12">
+      <c r="B16" s="3">
         <f>450*I1</f>
         <v>495.00000000000006</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C16" s="3" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B13">
-        <f>B12/F11</f>
-        <v>0.89090012330456247</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B14">
-        <f>I8/B13</f>
-        <v>0.29736666666666667</v>
-      </c>
-      <c r="D14">
-        <f>B11/B14</f>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="B15" s="22">
-        <f>F8/B13</f>
-        <v>2604.9319999999998</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B17">
+        <f>B16/F15</f>
+        <v>0.64820786683337073</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B18">
+        <f>I12/B17</f>
+        <v>0.29736666666666667</v>
+      </c>
+      <c r="D18">
+        <f>B15/B18</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="B19" s="22">
+        <f>F12/B17</f>
+        <v>2604.9320000000007</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B17">
+      <c r="B21">
         <v>30</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C21" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I23" t="s">
         <v>152</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J23" t="s">
         <v>153</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K23" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>138</v>
       </c>
-      <c r="B20">
+      <c r="B24">
         <f>61753*1000</f>
         <v>61753000</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C24" t="s">
         <v>141</v>
       </c>
-      <c r="D20">
+      <c r="D24">
         <v>20</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E24" t="s">
         <v>143</v>
       </c>
-      <c r="F20">
-        <f>B20/(D20*1000)</f>
+      <c r="F24">
+        <f>B24/(D24*1000)</f>
         <v>3087.65</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G24" t="s">
         <v>22</v>
       </c>
-      <c r="I20">
-        <f>B15/F21</f>
-        <v>73.44733082706766</v>
-      </c>
-      <c r="J20">
-        <f>B15/(F21+F20)</f>
-        <v>0.83408091276342533</v>
-      </c>
-      <c r="K20" s="15">
-        <f>F21/F20</f>
+      <c r="I24">
+        <f>B19/F25</f>
+        <v>73.447330827067688</v>
+      </c>
+      <c r="J24">
+        <f>F12/(F25+F24)</f>
+        <v>0.5406578092288109</v>
+      </c>
+      <c r="K24" s="15">
+        <f>F25/F24</f>
         <v>1.1486621432696928E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>139</v>
-      </c>
-      <c r="B21">
-        <v>1064000</v>
-      </c>
-      <c r="C21" t="s">
-        <v>141</v>
-      </c>
-      <c r="D21">
-        <v>30</v>
-      </c>
-      <c r="E21" t="s">
-        <v>143</v>
-      </c>
-      <c r="F21" s="2">
-        <f>B21/(D21*1000)</f>
-        <v>35.466666666666669</v>
-      </c>
-      <c r="G21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23">
-        <v>1089000</v>
-      </c>
-      <c r="C23" t="s">
-        <v>141</v>
-      </c>
-      <c r="D23">
-        <f>B23/1000000</f>
-        <v>1.089</v>
-      </c>
-      <c r="E23" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25">
+        <v>1064000</v>
+      </c>
+      <c r="C25" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25">
+        <v>30</v>
+      </c>
+      <c r="E25" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="2">
+        <f>B25/(D25*1000)</f>
+        <v>35.466666666666669</v>
+      </c>
+      <c r="G25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27">
+        <v>1089000</v>
+      </c>
+      <c r="C27" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27">
+        <f>B27/1000000</f>
+        <v>1.089</v>
+      </c>
+      <c r="E27" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>144</v>
       </c>
-      <c r="B25">
+      <c r="B29">
         <v>12</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C29" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B26">
-        <f>B25*(365*24*60*60)</f>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <f>B29*(365*24*60*60)</f>
         <v>378432000</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C30" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B27">
-        <f>B26*0.3</f>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <f>B30*0.3</f>
         <v>113529600</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C31" t="s">
         <v>110</v>
       </c>
-      <c r="D27">
-        <f>B27*G1/(1000000)</f>
+      <c r="D31">
+        <f>B31*G1/(1000000)</f>
         <v>1.0320872727272727</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E31" t="s">
         <v>145</v>
       </c>
-      <c r="F27">
-        <f>D27/I1</f>
+      <c r="F31">
+        <f>D31/I1</f>
         <v>0.93826115702479329</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G31" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B29">
-        <f>(B20/1000000)+F27</f>
+      <c r="B33">
+        <f>(B24/1000000)+F31</f>
         <v>62.69126115702479</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C33" t="s">
         <v>147</v>
       </c>
-      <c r="D29">
-        <f>B29*I1</f>
+      <c r="D33">
+        <f>B33*I1</f>
         <v>68.960387272727274</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E33" t="s">
         <v>145</v>
       </c>
-      <c r="F29" s="15">
-        <f>D29/B15</f>
-        <v>2.6473008613171967E-2</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="F33" s="15">
+        <f>D33/F12</f>
+        <v>4.084030751199931E-2</v>
+      </c>
+      <c r="G33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B32">
-        <f>D23</f>
+      <c r="B36">
+        <f>D27</f>
         <v>1.089</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C36" t="s">
         <v>147</v>
       </c>
-      <c r="D32">
-        <f>B32*I1</f>
+      <c r="D36">
+        <f>B36*I1</f>
         <v>1.1979</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E36" t="s">
         <v>145</v>
       </c>
-      <c r="F32" s="15">
-        <f>D32/B14</f>
-        <v>4.028360049321825</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="F36" s="15">
+        <f>D36/I12</f>
+        <v>6.214611477952583</v>
+      </c>
+      <c r="G36" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B35">
-        <f>F8*B17*1000</f>
-        <v>69622027.200000018</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B39">
+        <f>F12*B21*1000</f>
+        <v>50656122.448979594</v>
+      </c>
+      <c r="C39" t="s">
         <v>156</v>
       </c>
-      <c r="D35">
-        <f>D9/(B35/1000)</f>
-        <v>3.2613126783530364E-4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="D39">
+        <f>D13/(B39/1000)</f>
+        <v>4.4823644018290594E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B36">
-        <f>(B11*1000000)+(70005000*B17)</f>
+      <c r="B40">
+        <f>(B15*1000000)+(70005000*B21)</f>
         <v>2233965000</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C40" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="24" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="B37" s="22">
-        <f>B36/B35</f>
-        <v>32.08704327988886</v>
-      </c>
-      <c r="C37" s="22" t="s">
+      <c r="B41" s="22">
+        <f>B40/B39</f>
+        <v>44.100592228511573</v>
+      </c>
+      <c r="C41" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="D37" s="22"/>
+      <c r="D41" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added data for photoconversion
Former-commit-id: b3250cd2f825c7681060920db00a989d53d496b5
Former-commit-id: 0aeef458c683152f60caaa85f44c41c4286e0478
</commit_message>
<xml_diff>
--- a/data/i2cner-tech-data.xlsx
+++ b/data/i2cner-tech-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48FB379-1C6E-4F59-BBDC-19F34217ED84}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF8BB48-A49D-4892-9B2E-70D6B8B6F54E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
+    <workbookView xWindow="36000" yWindow="2625" windowWidth="21600" windowHeight="11325" firstSheet="7" activeTab="13" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CCS_Costs_Early" sheetId="14" r:id="rId1"/>
@@ -26,7 +26,8 @@
     <sheet name="Keipi_electrolysis" sheetId="8" r:id="rId11"/>
     <sheet name="Simons_PEMFC" sheetId="10" r:id="rId12"/>
     <sheet name="EIA_LCOE" sheetId="11" r:id="rId13"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId14"/>
+    <sheet name="Photoconversion" sheetId="16" r:id="rId14"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="292">
   <si>
     <t>H2 Method</t>
   </si>
@@ -818,6 +819,108 @@
   </si>
   <si>
     <t>Cap</t>
+  </si>
+  <si>
+    <t>Japan area</t>
+  </si>
+  <si>
+    <t>sq km</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>Solar cost</t>
+  </si>
+  <si>
+    <t>acres/MW</t>
+  </si>
+  <si>
+    <t>sq km/acre</t>
+  </si>
+  <si>
+    <t>sq km/GW</t>
+  </si>
+  <si>
+    <t>Solar land</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>kgH2/day</t>
+  </si>
+  <si>
+    <t>kgH2/year</t>
+  </si>
+  <si>
+    <t>kg/lifetime</t>
+  </si>
+  <si>
+    <t>Area cost</t>
+  </si>
+  <si>
+    <t>sqkm</t>
+  </si>
+  <si>
+    <t>% of forest</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Unit area cost</t>
+  </si>
+  <si>
+    <t>Area for photoH2</t>
+  </si>
+  <si>
+    <t>H2 cost</t>
+  </si>
+  <si>
+    <t>Correction factor</t>
+  </si>
+  <si>
+    <t>GWh/year</t>
+  </si>
+  <si>
+    <t>GWh/lifetime</t>
+  </si>
+  <si>
+    <t>Cap lim</t>
+  </si>
+  <si>
+    <t>Target:</t>
+  </si>
+  <si>
+    <t>$3/kgH2</t>
+  </si>
+  <si>
+    <t>$/kg-H2</t>
+  </si>
+  <si>
+    <t>MUSD/GW/year</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ijhydene.2010.12.035</t>
+  </si>
+  <si>
+    <t>LCA emissions</t>
+  </si>
+  <si>
+    <t>gCO2eq/kgH2</t>
+  </si>
+  <si>
+    <t>Emissions -Lb</t>
+  </si>
+  <si>
+    <t>Emissions -Ub</t>
+  </si>
+  <si>
+    <t>nuclear based</t>
+  </si>
+  <si>
+    <t>biomass</t>
   </si>
 </sst>
 </file>
@@ -1004,13 +1107,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1329,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3B25EB-4023-477D-80C4-74718858ACC8}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33:P44"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1383,15 +1486,15 @@
       <c r="C3" t="s">
         <v>190</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1881,15 +1984,15 @@
       <c r="C17" t="s">
         <v>251</v>
       </c>
-      <c r="J17" s="25" t="s">
+      <c r="J17" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -2351,15 +2454,15 @@
       <c r="E31">
         <v>0.7</v>
       </c>
-      <c r="J31" s="25" t="s">
+      <c r="J31" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="25"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="26"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -3851,10 +3954,10 @@
         <v>2025</v>
       </c>
       <c r="D3" s="18"/>
-      <c r="E3" s="25">
+      <c r="E3" s="26">
         <v>2040</v>
       </c>
-      <c r="F3" s="25"/>
+      <c r="F3" s="26"/>
       <c r="G3" t="s">
         <v>197</v>
       </c>
@@ -4103,6 +4206,341 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403B81F9-D657-42BD-96F8-D40A873BAE34}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1">
+        <v>377970</v>
+      </c>
+      <c r="C1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2">
+        <v>251000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3">
+        <v>7.5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>262</v>
+      </c>
+      <c r="I3">
+        <v>4.0468600000000002E-3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <f>B3*I3*1000</f>
+        <v>30.351450000000003</v>
+      </c>
+      <c r="C4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5">
+        <f>300*B4</f>
+        <v>9105.4350000000013</v>
+      </c>
+      <c r="C5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5">
+        <f>B5*100/B2</f>
+        <v>3.6276633466135464</v>
+      </c>
+      <c r="E5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>275</v>
+      </c>
+      <c r="B6">
+        <f>D6*B2/100</f>
+        <v>12550</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>277</v>
+      </c>
+      <c r="B8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11">
+        <v>1000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D11">
+        <f>365.25*B11*B9*B8</f>
+        <v>65745</v>
+      </c>
+      <c r="E11" t="s">
+        <v>268</v>
+      </c>
+      <c r="F11">
+        <f>D11*B10</f>
+        <v>1314900</v>
+      </c>
+      <c r="G11" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <f>30*D11/1000000</f>
+        <v>1.97235</v>
+      </c>
+      <c r="C12" t="s">
+        <v>278</v>
+      </c>
+      <c r="D12">
+        <f>B12*B10</f>
+        <v>39.447000000000003</v>
+      </c>
+      <c r="E12" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>270</v>
+      </c>
+      <c r="B13">
+        <f>222881/1000000</f>
+        <v>0.222881</v>
+      </c>
+      <c r="C13" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B14">
+        <f>B12/8760</f>
+        <v>2.2515410958904111E-4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>274</v>
+      </c>
+      <c r="B15">
+        <f>B13/B14</f>
+        <v>989.90420564301462</v>
+      </c>
+      <c r="C15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>280</v>
+      </c>
+      <c r="B16">
+        <f>B6/B15</f>
+        <v>12.67799442456946</v>
+      </c>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17">
+        <f>4.291722*1.3445</f>
+        <v>5.7702202290000004</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18">
+        <f>B17/B14</f>
+        <v>25627.869904449009</v>
+      </c>
+      <c r="C18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>276</v>
+      </c>
+      <c r="B19">
+        <f>(B17*1000000)/F11</f>
+        <v>4.3883338877481179</v>
+      </c>
+      <c r="C19" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" t="s">
+        <v>281</v>
+      </c>
+      <c r="F19" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20">
+        <f>F11*F20/(1000000*B10)</f>
+        <v>6.5744999999999998E-2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>284</v>
+      </c>
+      <c r="E20" t="s">
+        <v>281</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>286</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>288</v>
+      </c>
+      <c r="B25">
+        <v>411.8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>287</v>
+      </c>
+      <c r="E25">
+        <f>B25/30</f>
+        <v>13.726666666666667</v>
+      </c>
+      <c r="F25" t="s">
+        <v>129</v>
+      </c>
+      <c r="I25" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>289</v>
+      </c>
+      <c r="B26">
+        <v>3000</v>
+      </c>
+      <c r="C26" t="s">
+        <v>287</v>
+      </c>
+      <c r="E26">
+        <f>B26/30</f>
+        <v>100</v>
+      </c>
+      <c r="F26" t="s">
+        <v>129</v>
+      </c>
+      <c r="I26" t="s">
+        <v>291</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B23" r:id="rId1" tooltip="Persistent link using digital object identifier" xr:uid="{D7C525A3-6A36-47B4-A753-318099DBAD41}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E6C6BEB-6091-4743-A766-86BDD24D0263}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4174,15 +4612,15 @@
       <c r="C3" t="s">
         <v>190</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -4672,15 +5110,15 @@
       <c r="C17" t="s">
         <v>251</v>
       </c>
-      <c r="J17" s="25" t="s">
+      <c r="J17" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -5142,15 +5580,15 @@
       <c r="E31">
         <v>0.7</v>
       </c>
-      <c r="J31" s="25" t="s">
+      <c r="J31" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="25"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="26"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -5794,10 +6232,10 @@
       <c r="G10" t="s">
         <v>102</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="K10" s="26"/>
+      <c r="K10" s="27"/>
       <c r="L10" s="11">
         <f>L9/G5</f>
         <v>122583.35123523093</v>
@@ -5807,10 +6245,10 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="K11" s="26"/>
+      <c r="K11" s="27"/>
       <c r="L11" s="11">
         <f>M4*L10</f>
         <v>4086438.5967776584</v>
@@ -6984,7 +7422,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="25" t="s">
         <v>244</v>
       </c>
       <c r="B16" s="3">

</xml_diff>